<commit_message>
nambah harga untuk room vip dan munculkan detail paket untuk laporan transaksi
</commit_message>
<xml_diff>
--- a/datakomisiterapisbulanan.xlsx
+++ b/datakomisiterapisbulanan.xlsx
@@ -465,7 +465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H75"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="27.6" customWidth="1" min="4" max="4"/>
+    <col width="33.6" customWidth="1" min="4" max="4"/>
     <col width="15.6" customWidth="1" min="5" max="5"/>
     <col width="7.199999999999999" customWidth="1" min="6" max="6"/>
     <col width="14.4" customWidth="1" min="7" max="7"/>
@@ -500,7 +500,7 @@
     <row r="2" ht="30" customHeight="1">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>LAPORAN KOMISI TERAPIS BULAN 6 TAHUN 2025</t>
+          <t>LAPORAN KOMISI TERAPIS BULAN 7 TAHUN 2025</t>
         </is>
       </c>
       <c r="B2" s="4" t="n"/>
@@ -575,35 +575,35 @@
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
         <is>
-          <t>TF0051</t>
+          <t>TF0091</t>
         </is>
       </c>
       <c r="B6" s="6" t="inlineStr">
         <is>
-          <t>08-06-2025 19:37:51</t>
+          <t>06-07-2025 15:28:18</t>
         </is>
       </c>
       <c r="C6" s="6" t="inlineStr">
         <is>
-          <t>M003</t>
+          <t>M019</t>
         </is>
       </c>
       <c r="D6" s="6" t="inlineStr">
         <is>
-          <t>kalomania</t>
+          <t>Paket Jamail</t>
         </is>
       </c>
       <c r="E6" s="7" t="inlineStr">
         <is>
-          <t>500.000</t>
+          <t>350.000</t>
         </is>
       </c>
       <c r="F6" s="8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" s="7" t="inlineStr">
         <is>
-          <t>225.000</t>
+          <t>300.000</t>
         </is>
       </c>
       <c r="H6" s="6" t="inlineStr">
@@ -615,35 +615,35 @@
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
         <is>
-          <t>TF0057</t>
+          <t>TF0091</t>
         </is>
       </c>
       <c r="B7" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 14:02:33</t>
+          <t>06-07-2025 15:28:18</t>
         </is>
       </c>
       <c r="C7" s="6" t="inlineStr">
         <is>
-          <t>M002</t>
+          <t>P003</t>
         </is>
       </c>
       <c r="D7" s="6" t="inlineStr">
         <is>
-          <t>Paket Sejahteramana</t>
+          <t>Hot Stone</t>
         </is>
       </c>
       <c r="E7" s="7" t="inlineStr">
         <is>
-          <t>500.000</t>
+          <t>350.000</t>
         </is>
       </c>
       <c r="F7" s="8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="7" t="inlineStr">
         <is>
-          <t>400.000</t>
+          <t>70.000</t>
         </is>
       </c>
       <c r="H7" s="6" t="inlineStr">
@@ -655,27 +655,27 @@
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>TF0081</t>
+          <t>TF0091</t>
         </is>
       </c>
       <c r="B8" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 17:44:00</t>
+          <t>06-07-2025 15:28:18</t>
         </is>
       </c>
       <c r="C8" s="6" t="inlineStr">
         <is>
-          <t>M003</t>
+          <t>P001</t>
         </is>
       </c>
       <c r="D8" s="6" t="inlineStr">
         <is>
-          <t>kalomania</t>
+          <t>Traditional Massage 30 Min</t>
         </is>
       </c>
       <c r="E8" s="7" t="inlineStr">
         <is>
-          <t>500.000</t>
+          <t>200.000</t>
         </is>
       </c>
       <c r="F8" s="8" t="n">
@@ -683,7 +683,7 @@
       </c>
       <c r="G8" s="7" t="inlineStr">
         <is>
-          <t>225.000</t>
+          <t>20.000</t>
         </is>
       </c>
       <c r="H8" s="6" t="inlineStr">
@@ -695,12 +695,12 @@
     <row r="9">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>TF0082</t>
+          <t>TF0091</t>
         </is>
       </c>
       <c r="B9" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 17:47:24</t>
+          <t>06-07-2025 15:28:18</t>
         </is>
       </c>
       <c r="C9" s="6" t="inlineStr">
@@ -719,11 +719,11 @@
         </is>
       </c>
       <c r="F9" s="8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" s="7" t="inlineStr">
         <is>
-          <t>225.000</t>
+          <t>450.000</t>
         </is>
       </c>
       <c r="H9" s="6" t="inlineStr">
@@ -735,27 +735,27 @@
     <row r="10">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>TF0083</t>
+          <t>TF0093</t>
         </is>
       </c>
       <c r="B10" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 18:27:47</t>
+          <t>24-07-2025 22:34:21</t>
         </is>
       </c>
       <c r="C10" s="6" t="inlineStr">
         <is>
-          <t>M002</t>
+          <t>M001</t>
         </is>
       </c>
       <c r="D10" s="6" t="inlineStr">
         <is>
-          <t>Paket Sejahteramana</t>
+          <t>paket holiday</t>
         </is>
       </c>
       <c r="E10" s="7" t="inlineStr">
         <is>
-          <t>500.000</t>
+          <t>550.000</t>
         </is>
       </c>
       <c r="F10" s="8" t="n">
@@ -763,7 +763,7 @@
       </c>
       <c r="G10" s="7" t="inlineStr">
         <is>
-          <t>400.000</t>
+          <t>275.000</t>
         </is>
       </c>
       <c r="H10" s="6" t="inlineStr">
@@ -775,27 +775,27 @@
     <row r="11">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>TF0083</t>
+          <t>TF0094</t>
         </is>
       </c>
       <c r="B11" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 18:27:47</t>
+          <t>24-07-2025 23:04:19</t>
         </is>
       </c>
       <c r="C11" s="6" t="inlineStr">
         <is>
-          <t>M019</t>
+          <t>M002</t>
         </is>
       </c>
       <c r="D11" s="6" t="inlineStr">
         <is>
-          <t>Paket Jamail</t>
+          <t>Paket Sejahteramana</t>
         </is>
       </c>
       <c r="E11" s="7" t="inlineStr">
         <is>
-          <t>350.000</t>
+          <t>500.000</t>
         </is>
       </c>
       <c r="F11" s="8" t="n">
@@ -803,7 +803,7 @@
       </c>
       <c r="G11" s="7" t="inlineStr">
         <is>
-          <t>150.000</t>
+          <t>400.000</t>
         </is>
       </c>
       <c r="H11" s="6" t="inlineStr">
@@ -815,27 +815,27 @@
     <row r="12">
       <c r="A12" s="6" t="inlineStr">
         <is>
-          <t>TF0084</t>
+          <t>TF0095</t>
         </is>
       </c>
       <c r="B12" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 19:51:03</t>
+          <t>24-07-2025 23:11:22</t>
         </is>
       </c>
       <c r="C12" s="6" t="inlineStr">
         <is>
-          <t>M002</t>
+          <t>M001</t>
         </is>
       </c>
       <c r="D12" s="6" t="inlineStr">
         <is>
-          <t>Paket Sejahteramana</t>
+          <t>paket holiday</t>
         </is>
       </c>
       <c r="E12" s="7" t="inlineStr">
         <is>
-          <t>500.000</t>
+          <t>550.000</t>
         </is>
       </c>
       <c r="F12" s="8" t="n">
@@ -843,7 +843,7 @@
       </c>
       <c r="G12" s="7" t="inlineStr">
         <is>
-          <t>400.000</t>
+          <t>275.000</t>
         </is>
       </c>
       <c r="H12" s="6" t="inlineStr">
@@ -855,12 +855,12 @@
     <row r="13">
       <c r="A13" s="6" t="inlineStr">
         <is>
-          <t>TF0084</t>
+          <t>TF0100</t>
         </is>
       </c>
       <c r="B13" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 19:51:03</t>
+          <t>24-07-2025 23:33:28</t>
         </is>
       </c>
       <c r="C13" s="6" t="inlineStr">
@@ -895,27 +895,27 @@
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
         <is>
-          <t>TF0084</t>
+          <t>TF0102</t>
         </is>
       </c>
       <c r="B14" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 19:51:03</t>
+          <t>25-07-2025 00:37:55</t>
         </is>
       </c>
       <c r="C14" s="6" t="inlineStr">
         <is>
-          <t>M004</t>
+          <t>M002</t>
         </is>
       </c>
       <c r="D14" s="6" t="inlineStr">
         <is>
-          <t>paket bajinurakaloman</t>
+          <t>Paket Sejahteramana</t>
         </is>
       </c>
       <c r="E14" s="7" t="inlineStr">
         <is>
-          <t>4.000.000</t>
+          <t>500.000</t>
         </is>
       </c>
       <c r="F14" s="8" t="n">
@@ -933,144 +933,70 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="6" t="inlineStr">
-        <is>
-          <t>TF0087</t>
-        </is>
-      </c>
-      <c r="B15" s="6" t="inlineStr">
-        <is>
-          <t>16-06-2025 23:51:16</t>
-        </is>
-      </c>
-      <c r="C15" s="6" t="inlineStr">
-        <is>
-          <t>M003</t>
-        </is>
-      </c>
-      <c r="D15" s="6" t="inlineStr">
-        <is>
-          <t>kalomania</t>
-        </is>
-      </c>
-      <c r="E15" s="7" t="inlineStr">
-        <is>
-          <t>500.000</t>
-        </is>
-      </c>
-      <c r="F15" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G15" s="7" t="inlineStr">
-        <is>
-          <t>225.000</t>
-        </is>
-      </c>
-      <c r="H15" s="6" t="inlineStr">
-        <is>
-          <t>Lola</t>
-        </is>
-      </c>
+      <c r="A15" s="9" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="B15" s="6" t="n"/>
+      <c r="C15" s="6" t="n"/>
+      <c r="D15" s="6" t="n"/>
+      <c r="E15" s="6" t="n"/>
+      <c r="F15" s="9" t="inlineStr"/>
+      <c r="G15" s="10" t="inlineStr">
+        <is>
+          <t>2.415.000</t>
+        </is>
+      </c>
+      <c r="H15" s="9" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" s="6" t="inlineStr">
-        <is>
-          <t>TF0087</t>
-        </is>
-      </c>
-      <c r="B16" s="6" t="inlineStr">
-        <is>
-          <t>16-06-2025 23:51:16</t>
-        </is>
-      </c>
-      <c r="C16" s="6" t="inlineStr">
-        <is>
-          <t>M003</t>
-        </is>
-      </c>
-      <c r="D16" s="6" t="inlineStr">
-        <is>
-          <t>kalomania</t>
-        </is>
-      </c>
-      <c r="E16" s="7" t="inlineStr">
-        <is>
-          <t>500.000</t>
-        </is>
-      </c>
-      <c r="F16" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G16" s="7" t="inlineStr">
-        <is>
-          <t>225.000</t>
-        </is>
-      </c>
-      <c r="H16" s="6" t="inlineStr">
-        <is>
-          <t>Lola</t>
-        </is>
-      </c>
+      <c r="A16" s="6" t="n"/>
+      <c r="B16" s="6" t="n"/>
+      <c r="C16" s="6" t="n"/>
+      <c r="D16" s="6" t="n"/>
+      <c r="E16" s="6" t="n"/>
+      <c r="F16" s="6" t="n"/>
+      <c r="G16" s="6" t="n"/>
+      <c r="H16" s="6" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="6" t="inlineStr">
         <is>
-          <t>TF0087</t>
+          <t>Terapis :</t>
         </is>
       </c>
       <c r="B17" s="6" t="inlineStr">
         <is>
-          <t>16-06-2025 23:51:16</t>
-        </is>
-      </c>
-      <c r="C17" s="6" t="inlineStr">
-        <is>
-          <t>M002</t>
-        </is>
-      </c>
-      <c r="D17" s="6" t="inlineStr">
-        <is>
-          <t>Paket Sejahteramana</t>
-        </is>
-      </c>
-      <c r="E17" s="7" t="inlineStr">
-        <is>
-          <t>500.000</t>
-        </is>
-      </c>
-      <c r="F17" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G17" s="7" t="inlineStr">
-        <is>
-          <t>400.000</t>
-        </is>
-      </c>
-      <c r="H17" s="6" t="inlineStr">
-        <is>
-          <t>Lola</t>
-        </is>
-      </c>
+          <t>Sasa</t>
+        </is>
+      </c>
+      <c r="C17" s="6" t="n"/>
+      <c r="D17" s="6" t="n"/>
+      <c r="E17" s="6" t="n"/>
+      <c r="F17" s="6" t="n"/>
+      <c r="G17" s="6" t="n"/>
+      <c r="H17" s="6" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="6" t="inlineStr">
         <is>
-          <t>TF0088</t>
+          <t>TF0107</t>
         </is>
       </c>
       <c r="B18" s="6" t="inlineStr">
         <is>
-          <t>17-06-2025 11:29:14</t>
+          <t>26-07-2025 21:51:13</t>
         </is>
       </c>
       <c r="C18" s="6" t="inlineStr">
         <is>
-          <t>M002</t>
+          <t>M003</t>
         </is>
       </c>
       <c r="D18" s="6" t="inlineStr">
         <is>
-          <t>Paket Sejahteramana</t>
+          <t>kalomania</t>
         </is>
       </c>
       <c r="E18" s="7" t="inlineStr">
@@ -1083,34 +1009,34 @@
       </c>
       <c r="G18" s="7" t="inlineStr">
         <is>
-          <t>400.000</t>
+          <t>225.000</t>
         </is>
       </c>
       <c r="H18" s="6" t="inlineStr">
         <is>
-          <t>Lola</t>
+          <t>Sasa</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="6" t="inlineStr">
         <is>
-          <t>TF0089</t>
+          <t>TF0121</t>
         </is>
       </c>
       <c r="B19" s="6" t="inlineStr">
         <is>
-          <t>17-06-2025 11:37:15</t>
+          <t>27-07-2025 14:35:46</t>
         </is>
       </c>
       <c r="C19" s="6" t="inlineStr">
         <is>
-          <t>M002</t>
+          <t>M003</t>
         </is>
       </c>
       <c r="D19" s="6" t="inlineStr">
         <is>
-          <t>Paket Sejahteramana</t>
+          <t>kalomania</t>
         </is>
       </c>
       <c r="E19" s="7" t="inlineStr">
@@ -1119,124 +1045,198 @@
         </is>
       </c>
       <c r="F19" s="8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19" s="7" t="inlineStr">
         <is>
-          <t>400.000</t>
+          <t>450.000</t>
         </is>
       </c>
       <c r="H19" s="6" t="inlineStr">
         <is>
-          <t>Lola</t>
+          <t>Sasa</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="inlineStr">
         <is>
-          <t>TF0090</t>
+          <t>TF0125</t>
         </is>
       </c>
       <c r="B20" s="6" t="inlineStr">
         <is>
-          <t>17-06-2025 11:39:39</t>
+          <t>27-07-2025 14:55:07</t>
         </is>
       </c>
       <c r="C20" s="6" t="inlineStr">
         <is>
+          <t>M003</t>
+        </is>
+      </c>
+      <c r="D20" s="6" t="inlineStr">
+        <is>
+          <t>kalomania</t>
+        </is>
+      </c>
+      <c r="E20" s="7" t="inlineStr">
+        <is>
+          <t>500.000</t>
+        </is>
+      </c>
+      <c r="F20" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="7" t="inlineStr">
+        <is>
+          <t>225.000</t>
+        </is>
+      </c>
+      <c r="H20" s="6" t="inlineStr">
+        <is>
+          <t>Sasa</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>TF0141</t>
+        </is>
+      </c>
+      <c r="B21" s="6" t="inlineStr">
+        <is>
+          <t>27-07-2025 15:42:32</t>
+        </is>
+      </c>
+      <c r="C21" s="6" t="inlineStr">
+        <is>
+          <t>M006</t>
+        </is>
+      </c>
+      <c r="D21" s="6" t="inlineStr">
+        <is>
+          <t>paket lontong</t>
+        </is>
+      </c>
+      <c r="E21" s="7" t="inlineStr">
+        <is>
+          <t>6.550.000</t>
+        </is>
+      </c>
+      <c r="F21" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="7" t="inlineStr">
+        <is>
+          <t>150.000</t>
+        </is>
+      </c>
+      <c r="H21" s="6" t="inlineStr">
+        <is>
+          <t>Sasa</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="inlineStr">
+        <is>
+          <t>TF0145</t>
+        </is>
+      </c>
+      <c r="B22" s="6" t="inlineStr">
+        <is>
+          <t>27-07-2025 16:32:21</t>
+        </is>
+      </c>
+      <c r="C22" s="6" t="inlineStr">
+        <is>
           <t>M002</t>
         </is>
       </c>
-      <c r="D20" s="6" t="inlineStr">
+      <c r="D22" s="6" t="inlineStr">
         <is>
           <t>Paket Sejahteramana</t>
         </is>
       </c>
-      <c r="E20" s="7" t="inlineStr">
-        <is>
-          <t>500.000</t>
-        </is>
-      </c>
-      <c r="F20" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G20" s="7" t="inlineStr">
+      <c r="E22" s="7" t="inlineStr">
+        <is>
+          <t>500.000</t>
+        </is>
+      </c>
+      <c r="F22" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" s="7" t="inlineStr">
         <is>
           <t>400.000</t>
         </is>
       </c>
-      <c r="H20" s="6" t="inlineStr">
-        <is>
-          <t>Lola</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="9" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="B21" s="6" t="n"/>
-      <c r="C21" s="6" t="n"/>
-      <c r="D21" s="6" t="n"/>
-      <c r="E21" s="6" t="n"/>
-      <c r="F21" s="9" t="inlineStr"/>
-      <c r="G21" s="10" t="inlineStr">
-        <is>
-          <t>4.700.000</t>
-        </is>
-      </c>
-      <c r="H21" s="9" t="inlineStr"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="6" t="n"/>
-      <c r="B22" s="6" t="n"/>
-      <c r="C22" s="6" t="n"/>
-      <c r="D22" s="6" t="n"/>
-      <c r="E22" s="6" t="n"/>
-      <c r="F22" s="6" t="n"/>
-      <c r="G22" s="6" t="n"/>
-      <c r="H22" s="6" t="n"/>
+      <c r="H22" s="6" t="inlineStr">
+        <is>
+          <t>Sasa</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="6" t="inlineStr">
         <is>
-          <t>Terapis :</t>
+          <t>TF0145</t>
         </is>
       </c>
       <c r="B23" s="6" t="inlineStr">
         <is>
+          <t>27-07-2025 16:32:21</t>
+        </is>
+      </c>
+      <c r="C23" s="6" t="inlineStr">
+        <is>
+          <t>M002</t>
+        </is>
+      </c>
+      <c r="D23" s="6" t="inlineStr">
+        <is>
+          <t>Paket Sejahteramana</t>
+        </is>
+      </c>
+      <c r="E23" s="7" t="inlineStr">
+        <is>
+          <t>500.000</t>
+        </is>
+      </c>
+      <c r="F23" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" s="7" t="inlineStr">
+        <is>
+          <t>400.000</t>
+        </is>
+      </c>
+      <c r="H23" s="6" t="inlineStr">
+        <is>
           <t>Sasa</t>
         </is>
       </c>
-      <c r="C23" s="6" t="n"/>
-      <c r="D23" s="6" t="n"/>
-      <c r="E23" s="6" t="n"/>
-      <c r="F23" s="6" t="n"/>
-      <c r="G23" s="6" t="n"/>
-      <c r="H23" s="6" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="6" t="inlineStr">
         <is>
-          <t>TF0002</t>
+          <t>TF0150</t>
         </is>
       </c>
       <c r="B24" s="6" t="inlineStr">
         <is>
-          <t>06-06-2025 08:14:12</t>
+          <t>27-07-2025 16:43:36</t>
         </is>
       </c>
       <c r="C24" s="6" t="inlineStr">
         <is>
-          <t>M003</t>
+          <t>M002</t>
         </is>
       </c>
       <c r="D24" s="6" t="inlineStr">
         <is>
-          <t>kalomania</t>
+          <t>Paket Sejahteramana</t>
         </is>
       </c>
       <c r="E24" s="7" t="inlineStr">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="G24" s="7" t="inlineStr">
         <is>
-          <t>225.000</t>
+          <t>400.000</t>
         </is>
       </c>
       <c r="H24" s="6" t="inlineStr">
@@ -1261,12 +1261,12 @@
     <row r="25">
       <c r="A25" s="6" t="inlineStr">
         <is>
-          <t>TF0002</t>
+          <t>TF0155</t>
         </is>
       </c>
       <c r="B25" s="6" t="inlineStr">
         <is>
-          <t>06-06-2025 08:14:12</t>
+          <t>27-07-2025 16:58:10</t>
         </is>
       </c>
       <c r="C25" s="6" t="inlineStr">
@@ -1299,149 +1299,75 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="6" t="inlineStr">
-        <is>
-          <t>TF0002</t>
-        </is>
-      </c>
-      <c r="B26" s="6" t="inlineStr">
-        <is>
-          <t>06-06-2025 08:14:12</t>
-        </is>
-      </c>
-      <c r="C26" s="6" t="inlineStr">
-        <is>
-          <t>M003</t>
-        </is>
-      </c>
-      <c r="D26" s="6" t="inlineStr">
-        <is>
-          <t>kalomania</t>
-        </is>
-      </c>
-      <c r="E26" s="7" t="inlineStr">
-        <is>
-          <t>500.000</t>
-        </is>
-      </c>
-      <c r="F26" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G26" s="7" t="inlineStr">
-        <is>
-          <t>225.000</t>
-        </is>
-      </c>
-      <c r="H26" s="6" t="inlineStr">
-        <is>
-          <t>Sasa</t>
-        </is>
-      </c>
+      <c r="A26" s="9" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="B26" s="6" t="n"/>
+      <c r="C26" s="6" t="n"/>
+      <c r="D26" s="6" t="n"/>
+      <c r="E26" s="6" t="n"/>
+      <c r="F26" s="9" t="inlineStr"/>
+      <c r="G26" s="10" t="inlineStr">
+        <is>
+          <t>2.650.000</t>
+        </is>
+      </c>
+      <c r="H26" s="9" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" s="6" t="inlineStr">
-        <is>
-          <t>TF0002</t>
-        </is>
-      </c>
-      <c r="B27" s="6" t="inlineStr">
-        <is>
-          <t>06-06-2025 08:14:12</t>
-        </is>
-      </c>
-      <c r="C27" s="6" t="inlineStr">
-        <is>
-          <t>M002</t>
-        </is>
-      </c>
-      <c r="D27" s="6" t="inlineStr">
-        <is>
-          <t>Paket Sejahteramana</t>
-        </is>
-      </c>
-      <c r="E27" s="7" t="inlineStr">
-        <is>
-          <t>500.000</t>
-        </is>
-      </c>
-      <c r="F27" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G27" s="7" t="inlineStr">
-        <is>
-          <t>400.000</t>
-        </is>
-      </c>
-      <c r="H27" s="6" t="inlineStr">
-        <is>
-          <t>Sasa</t>
-        </is>
-      </c>
+      <c r="A27" s="6" t="n"/>
+      <c r="B27" s="6" t="n"/>
+      <c r="C27" s="6" t="n"/>
+      <c r="D27" s="6" t="n"/>
+      <c r="E27" s="6" t="n"/>
+      <c r="F27" s="6" t="n"/>
+      <c r="G27" s="6" t="n"/>
+      <c r="H27" s="6" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="6" t="inlineStr">
         <is>
-          <t>TF0002</t>
+          <t>Terapis :</t>
         </is>
       </c>
       <c r="B28" s="6" t="inlineStr">
         <is>
-          <t>06-06-2025 08:14:12</t>
-        </is>
-      </c>
-      <c r="C28" s="6" t="inlineStr">
-        <is>
-          <t>M003</t>
-        </is>
-      </c>
-      <c r="D28" s="6" t="inlineStr">
-        <is>
-          <t>kalomania</t>
-        </is>
-      </c>
-      <c r="E28" s="7" t="inlineStr">
-        <is>
-          <t>500.000</t>
-        </is>
-      </c>
-      <c r="F28" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G28" s="7" t="inlineStr">
-        <is>
-          <t>225.000</t>
-        </is>
-      </c>
-      <c r="H28" s="6" t="inlineStr">
-        <is>
-          <t>Sasa</t>
-        </is>
-      </c>
+          <t>Yola</t>
+        </is>
+      </c>
+      <c r="C28" s="6" t="n"/>
+      <c r="D28" s="6" t="n"/>
+      <c r="E28" s="6" t="n"/>
+      <c r="F28" s="6" t="n"/>
+      <c r="G28" s="6" t="n"/>
+      <c r="H28" s="6" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="6" t="inlineStr">
         <is>
-          <t>TF0003</t>
+          <t>TF0096</t>
         </is>
       </c>
       <c r="B29" s="6" t="inlineStr">
         <is>
-          <t>06-06-2025 08:45:33</t>
+          <t>24-07-2025 23:21:16</t>
         </is>
       </c>
       <c r="C29" s="6" t="inlineStr">
         <is>
-          <t>M004</t>
+          <t>M002</t>
         </is>
       </c>
       <c r="D29" s="6" t="inlineStr">
         <is>
-          <t>paket bajinurakaloman</t>
+          <t>Paket Sejahteramana</t>
         </is>
       </c>
       <c r="E29" s="7" t="inlineStr">
         <is>
-          <t>4.000.000</t>
+          <t>500.000</t>
         </is>
       </c>
       <c r="F29" s="8" t="n">
@@ -1454,34 +1380,34 @@
       </c>
       <c r="H29" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Yola</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="6" t="inlineStr">
         <is>
-          <t>TF0003</t>
+          <t>TF0097</t>
         </is>
       </c>
       <c r="B30" s="6" t="inlineStr">
         <is>
-          <t>06-06-2025 08:45:33</t>
+          <t>24-07-2025 23:27:44</t>
         </is>
       </c>
       <c r="C30" s="6" t="inlineStr">
         <is>
-          <t>M006</t>
+          <t>M002</t>
         </is>
       </c>
       <c r="D30" s="6" t="inlineStr">
         <is>
-          <t>paket lontong</t>
+          <t>Paket Sejahteramana</t>
         </is>
       </c>
       <c r="E30" s="7" t="inlineStr">
         <is>
-          <t>6.550.000</t>
+          <t>500.000</t>
         </is>
       </c>
       <c r="F30" s="8" t="n">
@@ -1489,74 +1415,74 @@
       </c>
       <c r="G30" s="7" t="inlineStr">
         <is>
-          <t>150.000</t>
+          <t>400.000</t>
         </is>
       </c>
       <c r="H30" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Yola</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="6" t="inlineStr">
         <is>
-          <t>TF0003</t>
+          <t>TF0099</t>
         </is>
       </c>
       <c r="B31" s="6" t="inlineStr">
         <is>
-          <t>06-06-2025 08:45:33</t>
+          <t>24-07-2025 23:32:11</t>
         </is>
       </c>
       <c r="C31" s="6" t="inlineStr">
         <is>
-          <t>M006</t>
+          <t>M002</t>
         </is>
       </c>
       <c r="D31" s="6" t="inlineStr">
         <is>
-          <t>paket lontong</t>
+          <t>Paket Sejahteramana</t>
         </is>
       </c>
       <c r="E31" s="7" t="inlineStr">
         <is>
-          <t>6.550.000</t>
+          <t>500.000</t>
         </is>
       </c>
       <c r="F31" s="8" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G31" s="7" t="inlineStr">
         <is>
-          <t>600.000</t>
+          <t>400.000</t>
         </is>
       </c>
       <c r="H31" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Yola</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="6" t="inlineStr">
         <is>
-          <t>TF0003</t>
+          <t>TF0101</t>
         </is>
       </c>
       <c r="B32" s="6" t="inlineStr">
         <is>
-          <t>06-06-2025 08:45:33</t>
+          <t>25-07-2025 00:31:08</t>
         </is>
       </c>
       <c r="C32" s="6" t="inlineStr">
         <is>
-          <t>M003</t>
+          <t>M002</t>
         </is>
       </c>
       <c r="D32" s="6" t="inlineStr">
         <is>
-          <t>kalomania</t>
+          <t>Paket Sejahteramana</t>
         </is>
       </c>
       <c r="E32" s="7" t="inlineStr">
@@ -1569,34 +1495,34 @@
       </c>
       <c r="G32" s="7" t="inlineStr">
         <is>
-          <t>225.000</t>
+          <t>400.000</t>
         </is>
       </c>
       <c r="H32" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Yola</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="6" t="inlineStr">
         <is>
-          <t>TF0003</t>
+          <t>TF0103</t>
         </is>
       </c>
       <c r="B33" s="6" t="inlineStr">
         <is>
-          <t>06-06-2025 08:45:33</t>
+          <t>25-07-2025 00:38:46</t>
         </is>
       </c>
       <c r="C33" s="6" t="inlineStr">
         <is>
-          <t>M002</t>
+          <t>M003</t>
         </is>
       </c>
       <c r="D33" s="6" t="inlineStr">
         <is>
-          <t>Paket Sejahteramana</t>
+          <t>kalomania</t>
         </is>
       </c>
       <c r="E33" s="7" t="inlineStr">
@@ -1609,64 +1535,64 @@
       </c>
       <c r="G33" s="7" t="inlineStr">
         <is>
-          <t>400.000</t>
+          <t>225.000</t>
         </is>
       </c>
       <c r="H33" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Yola</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="6" t="inlineStr">
         <is>
-          <t>TF0003</t>
+          <t>TF0105</t>
         </is>
       </c>
       <c r="B34" s="6" t="inlineStr">
         <is>
-          <t>06-06-2025 08:45:33</t>
+          <t>26-07-2025 21:49:18</t>
         </is>
       </c>
       <c r="C34" s="6" t="inlineStr">
         <is>
-          <t>M004</t>
+          <t>M002</t>
         </is>
       </c>
       <c r="D34" s="6" t="inlineStr">
         <is>
-          <t>paket bajinurakaloman</t>
+          <t>Paket Sejahteramana</t>
         </is>
       </c>
       <c r="E34" s="7" t="inlineStr">
         <is>
-          <t>4.000.000</t>
+          <t>500.000</t>
         </is>
       </c>
       <c r="F34" s="8" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G34" s="7" t="inlineStr">
         <is>
-          <t>1.200.000</t>
+          <t>400.000</t>
         </is>
       </c>
       <c r="H34" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Yola</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="6" t="inlineStr">
         <is>
-          <t>TF0003</t>
+          <t>TF0106</t>
         </is>
       </c>
       <c r="B35" s="6" t="inlineStr">
         <is>
-          <t>06-06-2025 08:45:33</t>
+          <t>26-07-2025 21:50:56</t>
         </is>
       </c>
       <c r="C35" s="6" t="inlineStr">
@@ -1694,19 +1620,19 @@
       </c>
       <c r="H35" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Yola</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="6" t="inlineStr">
         <is>
-          <t>TF0003</t>
+          <t>TF0108</t>
         </is>
       </c>
       <c r="B36" s="6" t="inlineStr">
         <is>
-          <t>06-06-2025 08:45:33</t>
+          <t>27-07-2025 13:21:52</t>
         </is>
       </c>
       <c r="C36" s="6" t="inlineStr">
@@ -1734,34 +1660,34 @@
       </c>
       <c r="H36" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Yola</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="6" t="inlineStr">
         <is>
-          <t>TF0004</t>
+          <t>TF0109</t>
         </is>
       </c>
       <c r="B37" s="6" t="inlineStr">
         <is>
-          <t>06-06-2025 08:48:47</t>
+          <t>27-07-2025 13:24:11</t>
         </is>
       </c>
       <c r="C37" s="6" t="inlineStr">
         <is>
-          <t>M007</t>
+          <t>M002</t>
         </is>
       </c>
       <c r="D37" s="6" t="inlineStr">
         <is>
-          <t>pasoaodkaosdoak</t>
+          <t>Paket Sejahteramana</t>
         </is>
       </c>
       <c r="E37" s="7" t="inlineStr">
         <is>
-          <t>600.000</t>
+          <t>500.000</t>
         </is>
       </c>
       <c r="F37" s="8" t="n">
@@ -1769,34 +1695,34 @@
       </c>
       <c r="G37" s="7" t="inlineStr">
         <is>
-          <t>1.500.000</t>
+          <t>400.000</t>
         </is>
       </c>
       <c r="H37" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Yola</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="6" t="inlineStr">
         <is>
-          <t>TF0004</t>
+          <t>TF0110</t>
         </is>
       </c>
       <c r="B38" s="6" t="inlineStr">
         <is>
-          <t>06-06-2025 08:48:47</t>
+          <t>27-07-2025 13:28:09</t>
         </is>
       </c>
       <c r="C38" s="6" t="inlineStr">
         <is>
-          <t>M002</t>
+          <t>M003</t>
         </is>
       </c>
       <c r="D38" s="6" t="inlineStr">
         <is>
-          <t>Paket Sejahteramana</t>
+          <t>kalomania</t>
         </is>
       </c>
       <c r="E38" s="7" t="inlineStr">
@@ -1805,43 +1731,43 @@
         </is>
       </c>
       <c r="F38" s="8" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G38" s="7" t="inlineStr">
         <is>
-          <t>1.600.000</t>
+          <t>225.000</t>
         </is>
       </c>
       <c r="H38" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Yola</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="6" t="inlineStr">
         <is>
-          <t>TF0004</t>
+          <t>TF0111</t>
         </is>
       </c>
       <c r="B39" s="6" t="inlineStr">
         <is>
-          <t>06-06-2025 08:48:47</t>
+          <t>27-07-2025 13:29:35</t>
         </is>
       </c>
       <c r="C39" s="6" t="inlineStr">
         <is>
-          <t>M006</t>
+          <t>M003</t>
         </is>
       </c>
       <c r="D39" s="6" t="inlineStr">
         <is>
-          <t>paket lontong</t>
+          <t>kalomania</t>
         </is>
       </c>
       <c r="E39" s="7" t="inlineStr">
         <is>
-          <t>6.550.000</t>
+          <t>500.000</t>
         </is>
       </c>
       <c r="F39" s="8" t="n">
@@ -1849,154 +1775,154 @@
       </c>
       <c r="G39" s="7" t="inlineStr">
         <is>
-          <t>150.000</t>
+          <t>225.000</t>
         </is>
       </c>
       <c r="H39" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Yola</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="6" t="inlineStr">
         <is>
-          <t>TF0004</t>
+          <t>TF0112</t>
         </is>
       </c>
       <c r="B40" s="6" t="inlineStr">
         <is>
-          <t>06-06-2025 08:48:47</t>
+          <t>27-07-2025 13:35:17</t>
         </is>
       </c>
       <c r="C40" s="6" t="inlineStr">
         <is>
-          <t>M006</t>
+          <t>M004</t>
         </is>
       </c>
       <c r="D40" s="6" t="inlineStr">
         <is>
-          <t>paket lontong</t>
+          <t>paket bajinurakaloman</t>
         </is>
       </c>
       <c r="E40" s="7" t="inlineStr">
         <is>
-          <t>6.550.000</t>
+          <t>4.000.000</t>
         </is>
       </c>
       <c r="F40" s="8" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G40" s="7" t="inlineStr">
         <is>
-          <t>600.000</t>
+          <t>400.000</t>
         </is>
       </c>
       <c r="H40" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Yola</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="6" t="inlineStr">
         <is>
-          <t>TF0004</t>
+          <t>TF0113</t>
         </is>
       </c>
       <c r="B41" s="6" t="inlineStr">
         <is>
-          <t>06-06-2025 08:48:47</t>
+          <t>27-07-2025 13:37:50</t>
         </is>
       </c>
       <c r="C41" s="6" t="inlineStr">
         <is>
-          <t>M004</t>
+          <t>M002</t>
         </is>
       </c>
       <c r="D41" s="6" t="inlineStr">
         <is>
-          <t>paket bajinurakaloman</t>
+          <t>Paket Sejahteramana</t>
         </is>
       </c>
       <c r="E41" s="7" t="inlineStr">
         <is>
-          <t>4.000.000</t>
+          <t>500.000</t>
         </is>
       </c>
       <c r="F41" s="8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G41" s="7" t="inlineStr">
         <is>
-          <t>800.000</t>
+          <t>400.000</t>
         </is>
       </c>
       <c r="H41" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Yola</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="6" t="inlineStr">
         <is>
-          <t>TF0004</t>
+          <t>TF0114</t>
         </is>
       </c>
       <c r="B42" s="6" t="inlineStr">
         <is>
-          <t>06-06-2025 08:48:47</t>
+          <t>27-07-2025 13:38:50</t>
         </is>
       </c>
       <c r="C42" s="6" t="inlineStr">
         <is>
-          <t>M004</t>
+          <t>M002</t>
         </is>
       </c>
       <c r="D42" s="6" t="inlineStr">
         <is>
-          <t>paket bajinurakaloman</t>
+          <t>Paket Sejahteramana</t>
         </is>
       </c>
       <c r="E42" s="7" t="inlineStr">
         <is>
-          <t>4.000.000</t>
+          <t>500.000</t>
         </is>
       </c>
       <c r="F42" s="8" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G42" s="7" t="inlineStr">
         <is>
-          <t>2.000.000</t>
+          <t>400.000</t>
         </is>
       </c>
       <c r="H42" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Yola</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="6" t="inlineStr">
         <is>
-          <t>TF0004</t>
+          <t>TF0115</t>
         </is>
       </c>
       <c r="B43" s="6" t="inlineStr">
         <is>
-          <t>06-06-2025 08:48:47</t>
+          <t>27-07-2025 14:00:35</t>
         </is>
       </c>
       <c r="C43" s="6" t="inlineStr">
         <is>
-          <t>M003</t>
+          <t>M002</t>
         </is>
       </c>
       <c r="D43" s="6" t="inlineStr">
         <is>
-          <t>kalomania</t>
+          <t>Paket Sejahteramana</t>
         </is>
       </c>
       <c r="E43" s="7" t="inlineStr">
@@ -2009,39 +1935,39 @@
       </c>
       <c r="G43" s="7" t="inlineStr">
         <is>
-          <t>225.000</t>
+          <t>400.000</t>
         </is>
       </c>
       <c r="H43" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Yola</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="6" t="inlineStr">
         <is>
-          <t>TF0004</t>
+          <t>TF0116</t>
         </is>
       </c>
       <c r="B44" s="6" t="inlineStr">
         <is>
-          <t>06-06-2025 08:48:47</t>
+          <t>27-07-2025 14:05:50</t>
         </is>
       </c>
       <c r="C44" s="6" t="inlineStr">
         <is>
-          <t>M002</t>
+          <t>M006</t>
         </is>
       </c>
       <c r="D44" s="6" t="inlineStr">
         <is>
-          <t>Paket Sejahteramana</t>
+          <t>paket lontong</t>
         </is>
       </c>
       <c r="E44" s="7" t="inlineStr">
         <is>
-          <t>500.000</t>
+          <t>6.550.000</t>
         </is>
       </c>
       <c r="F44" s="8" t="n">
@@ -2049,34 +1975,34 @@
       </c>
       <c r="G44" s="7" t="inlineStr">
         <is>
-          <t>400.000</t>
+          <t>150.000</t>
         </is>
       </c>
       <c r="H44" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Yola</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="6" t="inlineStr">
         <is>
-          <t>TF0053</t>
+          <t>TF0116</t>
         </is>
       </c>
       <c r="B45" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 12:58:55</t>
+          <t>27-07-2025 14:05:50</t>
         </is>
       </c>
       <c r="C45" s="6" t="inlineStr">
         <is>
-          <t>M003</t>
+          <t>M002</t>
         </is>
       </c>
       <c r="D45" s="6" t="inlineStr">
         <is>
-          <t>kalomania</t>
+          <t>Paket Sejahteramana</t>
         </is>
       </c>
       <c r="E45" s="7" t="inlineStr">
@@ -2089,39 +2015,39 @@
       </c>
       <c r="G45" s="7" t="inlineStr">
         <is>
-          <t>225.000</t>
+          <t>400.000</t>
         </is>
       </c>
       <c r="H45" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Yola</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="6" t="inlineStr">
         <is>
-          <t>TF0056</t>
+          <t>TF0116</t>
         </is>
       </c>
       <c r="B46" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 13:59:33</t>
+          <t>27-07-2025 14:05:50</t>
         </is>
       </c>
       <c r="C46" s="6" t="inlineStr">
         <is>
-          <t>M002</t>
+          <t>M008</t>
         </is>
       </c>
       <c r="D46" s="6" t="inlineStr">
         <is>
-          <t>Paket Sejahteramana</t>
+          <t>lasmladamaldk</t>
         </is>
       </c>
       <c r="E46" s="7" t="inlineStr">
         <is>
-          <t>500.000</t>
+          <t>5.000.000</t>
         </is>
       </c>
       <c r="F46" s="8" t="n">
@@ -2129,34 +2055,34 @@
       </c>
       <c r="G46" s="7" t="inlineStr">
         <is>
-          <t>400.000</t>
+          <t>150.000</t>
         </is>
       </c>
       <c r="H46" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Yola</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="6" t="inlineStr">
         <is>
-          <t>TF0058</t>
+          <t>TF0120</t>
         </is>
       </c>
       <c r="B47" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 14:05:31</t>
+          <t>27-07-2025 14:32:49</t>
         </is>
       </c>
       <c r="C47" s="6" t="inlineStr">
         <is>
-          <t>M002</t>
+          <t>M003</t>
         </is>
       </c>
       <c r="D47" s="6" t="inlineStr">
         <is>
-          <t>Paket Sejahteramana</t>
+          <t>kalomania</t>
         </is>
       </c>
       <c r="E47" s="7" t="inlineStr">
@@ -2169,34 +2095,34 @@
       </c>
       <c r="G47" s="7" t="inlineStr">
         <is>
-          <t>400.000</t>
+          <t>225.000</t>
         </is>
       </c>
       <c r="H47" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Yola</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="6" t="inlineStr">
         <is>
-          <t>TF0064</t>
+          <t>TF0124</t>
         </is>
       </c>
       <c r="B48" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 14:27:59</t>
+          <t>27-07-2025 14:48:51</t>
         </is>
       </c>
       <c r="C48" s="6" t="inlineStr">
         <is>
-          <t>M003</t>
+          <t>M002</t>
         </is>
       </c>
       <c r="D48" s="6" t="inlineStr">
         <is>
-          <t>kalomania</t>
+          <t>Paket Sejahteramana</t>
         </is>
       </c>
       <c r="E48" s="7" t="inlineStr">
@@ -2209,39 +2135,39 @@
       </c>
       <c r="G48" s="7" t="inlineStr">
         <is>
-          <t>225.000</t>
+          <t>400.000</t>
         </is>
       </c>
       <c r="H48" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Yola</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="6" t="inlineStr">
         <is>
-          <t>TF0073</t>
+          <t>TF0129</t>
         </is>
       </c>
       <c r="B49" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 14:52:39</t>
+          <t>27-07-2025 15:15:52</t>
         </is>
       </c>
       <c r="C49" s="6" t="inlineStr">
         <is>
-          <t>M019</t>
+          <t>M003</t>
         </is>
       </c>
       <c r="D49" s="6" t="inlineStr">
         <is>
-          <t>Paket Jamail</t>
+          <t>kalomania</t>
         </is>
       </c>
       <c r="E49" s="7" t="inlineStr">
         <is>
-          <t>350.000</t>
+          <t>500.000</t>
         </is>
       </c>
       <c r="F49" s="8" t="n">
@@ -2249,70 +2175,144 @@
       </c>
       <c r="G49" s="7" t="inlineStr">
         <is>
-          <t>150.000</t>
+          <t>225.000</t>
         </is>
       </c>
       <c r="H49" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Yola</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="9" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="B50" s="6" t="n"/>
-      <c r="C50" s="6" t="n"/>
-      <c r="D50" s="6" t="n"/>
-      <c r="E50" s="6" t="n"/>
-      <c r="F50" s="9" t="inlineStr"/>
-      <c r="G50" s="10" t="inlineStr">
-        <is>
-          <t>13.750.000</t>
-        </is>
-      </c>
-      <c r="H50" s="9" t="inlineStr"/>
+      <c r="A50" s="6" t="inlineStr">
+        <is>
+          <t>TF0130</t>
+        </is>
+      </c>
+      <c r="B50" s="6" t="inlineStr">
+        <is>
+          <t>27-07-2025 15:17:35</t>
+        </is>
+      </c>
+      <c r="C50" s="6" t="inlineStr">
+        <is>
+          <t>M002</t>
+        </is>
+      </c>
+      <c r="D50" s="6" t="inlineStr">
+        <is>
+          <t>Paket Sejahteramana</t>
+        </is>
+      </c>
+      <c r="E50" s="7" t="inlineStr">
+        <is>
+          <t>500.000</t>
+        </is>
+      </c>
+      <c r="F50" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G50" s="7" t="inlineStr">
+        <is>
+          <t>400.000</t>
+        </is>
+      </c>
+      <c r="H50" s="6" t="inlineStr">
+        <is>
+          <t>Yola</t>
+        </is>
+      </c>
     </row>
     <row r="51">
-      <c r="A51" s="6" t="n"/>
-      <c r="B51" s="6" t="n"/>
-      <c r="C51" s="6" t="n"/>
-      <c r="D51" s="6" t="n"/>
-      <c r="E51" s="6" t="n"/>
-      <c r="F51" s="6" t="n"/>
-      <c r="G51" s="6" t="n"/>
-      <c r="H51" s="6" t="n"/>
+      <c r="A51" s="6" t="inlineStr">
+        <is>
+          <t>TF0133</t>
+        </is>
+      </c>
+      <c r="B51" s="6" t="inlineStr">
+        <is>
+          <t>27-07-2025 15:25:00</t>
+        </is>
+      </c>
+      <c r="C51" s="6" t="inlineStr">
+        <is>
+          <t>M002</t>
+        </is>
+      </c>
+      <c r="D51" s="6" t="inlineStr">
+        <is>
+          <t>Paket Sejahteramana</t>
+        </is>
+      </c>
+      <c r="E51" s="7" t="inlineStr">
+        <is>
+          <t>500.000</t>
+        </is>
+      </c>
+      <c r="F51" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G51" s="7" t="inlineStr">
+        <is>
+          <t>400.000</t>
+        </is>
+      </c>
+      <c r="H51" s="6" t="inlineStr">
+        <is>
+          <t>Yola</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="6" t="inlineStr">
         <is>
-          <t>Terapis :</t>
+          <t>TF0134</t>
         </is>
       </c>
       <c r="B52" s="6" t="inlineStr">
         <is>
-          <t>Yola</t>
-        </is>
-      </c>
-      <c r="C52" s="6" t="n"/>
-      <c r="D52" s="6" t="n"/>
-      <c r="E52" s="6" t="n"/>
-      <c r="F52" s="6" t="n"/>
-      <c r="G52" s="6" t="n"/>
-      <c r="H52" s="6" t="n"/>
+          <t>27-07-2025 15:26:58</t>
+        </is>
+      </c>
+      <c r="C52" s="6" t="inlineStr">
+        <is>
+          <t>M003</t>
+        </is>
+      </c>
+      <c r="D52" s="6" t="inlineStr">
+        <is>
+          <t>kalomania</t>
+        </is>
+      </c>
+      <c r="E52" s="7" t="inlineStr">
+        <is>
+          <t>500.000</t>
+        </is>
+      </c>
+      <c r="F52" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G52" s="7" t="inlineStr">
+        <is>
+          <t>225.000</t>
+        </is>
+      </c>
+      <c r="H52" s="6" t="inlineStr">
+        <is>
+          <t>Yola</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="6" t="inlineStr">
         <is>
-          <t>TF0052</t>
+          <t>TF0137</t>
         </is>
       </c>
       <c r="B53" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 12:51:24</t>
+          <t>27-07-2025 15:36:17</t>
         </is>
       </c>
       <c r="C53" s="6" t="inlineStr">
@@ -2347,27 +2347,27 @@
     <row r="54">
       <c r="A54" s="6" t="inlineStr">
         <is>
-          <t>TF0055</t>
+          <t>TF0142</t>
         </is>
       </c>
       <c r="B54" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 13:57:05</t>
+          <t>27-07-2025 16:26:27</t>
         </is>
       </c>
       <c r="C54" s="6" t="inlineStr">
         <is>
-          <t>M001</t>
+          <t>M002</t>
         </is>
       </c>
       <c r="D54" s="6" t="inlineStr">
         <is>
-          <t>paket holiday</t>
+          <t>Paket Sejahteramana</t>
         </is>
       </c>
       <c r="E54" s="7" t="inlineStr">
         <is>
-          <t>550.000</t>
+          <t>500.000</t>
         </is>
       </c>
       <c r="F54" s="8" t="n">
@@ -2375,7 +2375,7 @@
       </c>
       <c r="G54" s="7" t="inlineStr">
         <is>
-          <t>275.000</t>
+          <t>400.000</t>
         </is>
       </c>
       <c r="H54" s="6" t="inlineStr">
@@ -2387,27 +2387,27 @@
     <row r="55">
       <c r="A55" s="6" t="inlineStr">
         <is>
-          <t>TF0059</t>
+          <t>TF0144</t>
         </is>
       </c>
       <c r="B55" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 14:12:46</t>
+          <t>27-07-2025 16:31:07</t>
         </is>
       </c>
       <c r="C55" s="6" t="inlineStr">
         <is>
-          <t>M002</t>
+          <t>M001</t>
         </is>
       </c>
       <c r="D55" s="6" t="inlineStr">
         <is>
-          <t>Paket Sejahteramana</t>
+          <t>paket holiday</t>
         </is>
       </c>
       <c r="E55" s="7" t="inlineStr">
         <is>
-          <t>500.000</t>
+          <t>550.000</t>
         </is>
       </c>
       <c r="F55" s="8" t="n">
@@ -2415,7 +2415,7 @@
       </c>
       <c r="G55" s="7" t="inlineStr">
         <is>
-          <t>400.000</t>
+          <t>275.000</t>
         </is>
       </c>
       <c r="H55" s="6" t="inlineStr">
@@ -2427,12 +2427,12 @@
     <row r="56">
       <c r="A56" s="6" t="inlineStr">
         <is>
-          <t>TF0060</t>
+          <t>TF0149</t>
         </is>
       </c>
       <c r="B56" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 14:17:53</t>
+          <t>27-07-2025 16:39:27</t>
         </is>
       </c>
       <c r="C56" s="6" t="inlineStr">
@@ -2467,22 +2467,22 @@
     <row r="57">
       <c r="A57" s="6" t="inlineStr">
         <is>
-          <t>TF0061</t>
+          <t>TF0154</t>
         </is>
       </c>
       <c r="B57" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 14:21:05</t>
+          <t>27-07-2025 16:56:27</t>
         </is>
       </c>
       <c r="C57" s="6" t="inlineStr">
         <is>
-          <t>M003</t>
+          <t>M002</t>
         </is>
       </c>
       <c r="D57" s="6" t="inlineStr">
         <is>
-          <t>kalomania</t>
+          <t>Paket Sejahteramana</t>
         </is>
       </c>
       <c r="E57" s="7" t="inlineStr">
@@ -2495,7 +2495,7 @@
       </c>
       <c r="G57" s="7" t="inlineStr">
         <is>
-          <t>225.000</t>
+          <t>400.000</t>
         </is>
       </c>
       <c r="H57" s="6" t="inlineStr">
@@ -2507,22 +2507,22 @@
     <row r="58">
       <c r="A58" s="6" t="inlineStr">
         <is>
-          <t>TF0062</t>
+          <t>TF0157</t>
         </is>
       </c>
       <c r="B58" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 14:23:54</t>
+          <t>29-07-2025 12:05:08</t>
         </is>
       </c>
       <c r="C58" s="6" t="inlineStr">
         <is>
-          <t>M003</t>
+          <t>M002</t>
         </is>
       </c>
       <c r="D58" s="6" t="inlineStr">
         <is>
-          <t>kalomania</t>
+          <t>Paket Sejahteramana</t>
         </is>
       </c>
       <c r="E58" s="7" t="inlineStr">
@@ -2535,7 +2535,7 @@
       </c>
       <c r="G58" s="7" t="inlineStr">
         <is>
-          <t>225.000</t>
+          <t>400.000</t>
         </is>
       </c>
       <c r="H58" s="6" t="inlineStr">
@@ -2547,27 +2547,27 @@
     <row r="59">
       <c r="A59" s="6" t="inlineStr">
         <is>
-          <t>TF0063</t>
+          <t>TF0157</t>
         </is>
       </c>
       <c r="B59" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 14:25:36</t>
+          <t>29-07-2025 12:05:08</t>
         </is>
       </c>
       <c r="C59" s="6" t="inlineStr">
         <is>
-          <t>M002</t>
+          <t>P002</t>
         </is>
       </c>
       <c r="D59" s="6" t="inlineStr">
         <is>
-          <t>Paket Sejahteramana</t>
+          <t>Hot Massage</t>
         </is>
       </c>
       <c r="E59" s="7" t="inlineStr">
         <is>
-          <t>500.000</t>
+          <t>300.000</t>
         </is>
       </c>
       <c r="F59" s="8" t="n">
@@ -2575,7 +2575,7 @@
       </c>
       <c r="G59" s="7" t="inlineStr">
         <is>
-          <t>400.000</t>
+          <t>30.000</t>
         </is>
       </c>
       <c r="H59" s="6" t="inlineStr">
@@ -2587,27 +2587,27 @@
     <row r="60">
       <c r="A60" s="6" t="inlineStr">
         <is>
-          <t>TF0065</t>
+          <t>TF0157</t>
         </is>
       </c>
       <c r="B60" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 14:29:12</t>
+          <t>29-07-2025 12:05:08</t>
         </is>
       </c>
       <c r="C60" s="6" t="inlineStr">
         <is>
-          <t>M019</t>
+          <t>P001</t>
         </is>
       </c>
       <c r="D60" s="6" t="inlineStr">
         <is>
-          <t>Paket Jamail</t>
+          <t>Traditional Massage 30 Min</t>
         </is>
       </c>
       <c r="E60" s="7" t="inlineStr">
         <is>
-          <t>350.000</t>
+          <t>200.000</t>
         </is>
       </c>
       <c r="F60" s="8" t="n">
@@ -2615,7 +2615,7 @@
       </c>
       <c r="G60" s="7" t="inlineStr">
         <is>
-          <t>150.000</t>
+          <t>20.000</t>
         </is>
       </c>
       <c r="H60" s="6" t="inlineStr">
@@ -2627,22 +2627,22 @@
     <row r="61">
       <c r="A61" s="6" t="inlineStr">
         <is>
-          <t>TF0066</t>
+          <t>TF0157</t>
         </is>
       </c>
       <c r="B61" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 14:30:00</t>
+          <t>29-07-2025 12:05:08</t>
         </is>
       </c>
       <c r="C61" s="6" t="inlineStr">
         <is>
-          <t>M002</t>
+          <t>M003</t>
         </is>
       </c>
       <c r="D61" s="6" t="inlineStr">
         <is>
-          <t>Paket Sejahteramana</t>
+          <t>kalomania</t>
         </is>
       </c>
       <c r="E61" s="7" t="inlineStr">
@@ -2655,7 +2655,7 @@
       </c>
       <c r="G61" s="7" t="inlineStr">
         <is>
-          <t>400.000</t>
+          <t>225.000</t>
         </is>
       </c>
       <c r="H61" s="6" t="inlineStr">
@@ -2667,22 +2667,22 @@
     <row r="62">
       <c r="A62" s="6" t="inlineStr">
         <is>
-          <t>TF0067</t>
+          <t>TF0157</t>
         </is>
       </c>
       <c r="B62" s="6" t="inlineStr">
         <is>
-          <t>15-06-2025 14:31:00</t>
+          <t>29-07-2025 12:05:08</t>
         </is>
       </c>
       <c r="C62" s="6" t="inlineStr">
         <is>
-          <t>M003</t>
+          <t>M002</t>
         </is>
       </c>
       <c r="D62" s="6" t="inlineStr">
         <is>
-          <t>kalomania</t>
+          <t>Paket Sejahteramana</t>
         </is>
       </c>
       <c r="E62" s="7" t="inlineStr">
@@ -2695,7 +2695,7 @@
       </c>
       <c r="G62" s="7" t="inlineStr">
         <is>
-          <t>225.000</t>
+          <t>400.000</t>
         </is>
       </c>
       <c r="H62" s="6" t="inlineStr">
@@ -2705,408 +2705,48 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="6" t="inlineStr">
-        <is>
-          <t>TF0068</t>
-        </is>
-      </c>
-      <c r="B63" s="6" t="inlineStr">
-        <is>
-          <t>15-06-2025 14:33:27</t>
-        </is>
-      </c>
-      <c r="C63" s="6" t="inlineStr">
-        <is>
-          <t>M019</t>
-        </is>
-      </c>
-      <c r="D63" s="6" t="inlineStr">
-        <is>
-          <t>Paket Jamail</t>
-        </is>
-      </c>
-      <c r="E63" s="7" t="inlineStr">
-        <is>
-          <t>350.000</t>
-        </is>
-      </c>
-      <c r="F63" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G63" s="7" t="inlineStr">
-        <is>
-          <t>150.000</t>
-        </is>
-      </c>
-      <c r="H63" s="6" t="inlineStr">
-        <is>
-          <t>Yola</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="6" t="inlineStr">
-        <is>
-          <t>TF0069</t>
-        </is>
-      </c>
-      <c r="B64" s="6" t="inlineStr">
-        <is>
-          <t>15-06-2025 14:35:15</t>
-        </is>
-      </c>
-      <c r="C64" s="6" t="inlineStr">
-        <is>
-          <t>M019</t>
-        </is>
-      </c>
-      <c r="D64" s="6" t="inlineStr">
-        <is>
-          <t>Paket Jamail</t>
-        </is>
-      </c>
-      <c r="E64" s="7" t="inlineStr">
-        <is>
-          <t>350.000</t>
-        </is>
-      </c>
-      <c r="F64" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G64" s="7" t="inlineStr">
-        <is>
-          <t>150.000</t>
-        </is>
-      </c>
-      <c r="H64" s="6" t="inlineStr">
-        <is>
-          <t>Yola</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="6" t="inlineStr">
-        <is>
-          <t>TF0071</t>
-        </is>
-      </c>
-      <c r="B65" s="6" t="inlineStr">
-        <is>
-          <t>15-06-2025 14:46:23</t>
-        </is>
-      </c>
-      <c r="C65" s="6" t="inlineStr">
-        <is>
-          <t>M019</t>
-        </is>
-      </c>
-      <c r="D65" s="6" t="inlineStr">
-        <is>
-          <t>Paket Jamail</t>
-        </is>
-      </c>
-      <c r="E65" s="7" t="inlineStr">
-        <is>
-          <t>350.000</t>
-        </is>
-      </c>
-      <c r="F65" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G65" s="7" t="inlineStr">
-        <is>
-          <t>150.000</t>
-        </is>
-      </c>
-      <c r="H65" s="6" t="inlineStr">
-        <is>
-          <t>Yola</t>
-        </is>
-      </c>
+      <c r="A63" s="9" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="B63" s="6" t="n"/>
+      <c r="C63" s="6" t="n"/>
+      <c r="D63" s="6" t="n"/>
+      <c r="E63" s="6" t="n"/>
+      <c r="F63" s="9" t="inlineStr"/>
+      <c r="G63" s="10" t="inlineStr">
+        <is>
+          <t>10.825.000</t>
+        </is>
+      </c>
+      <c r="H63" s="9" t="inlineStr"/>
     </row>
     <row r="66">
-      <c r="A66" s="6" t="inlineStr">
-        <is>
-          <t>TF0072</t>
-        </is>
-      </c>
-      <c r="B66" s="6" t="inlineStr">
-        <is>
-          <t>15-06-2025 14:51:13</t>
-        </is>
-      </c>
-      <c r="C66" s="6" t="inlineStr">
-        <is>
-          <t>M003</t>
-        </is>
-      </c>
-      <c r="D66" s="6" t="inlineStr">
-        <is>
-          <t>kalomania</t>
-        </is>
-      </c>
-      <c r="E66" s="7" t="inlineStr">
-        <is>
-          <t>500.000</t>
-        </is>
-      </c>
-      <c r="F66" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G66" s="7" t="inlineStr">
-        <is>
-          <t>225.000</t>
-        </is>
-      </c>
-      <c r="H66" s="6" t="inlineStr">
-        <is>
-          <t>Yola</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="6" t="inlineStr">
-        <is>
-          <t>TF0074</t>
-        </is>
-      </c>
-      <c r="B67" s="6" t="inlineStr">
-        <is>
-          <t>15-06-2025 15:05:29</t>
-        </is>
-      </c>
-      <c r="C67" s="6" t="inlineStr">
-        <is>
-          <t>M019</t>
-        </is>
-      </c>
-      <c r="D67" s="6" t="inlineStr">
-        <is>
-          <t>Paket Jamail</t>
-        </is>
-      </c>
-      <c r="E67" s="7" t="inlineStr">
-        <is>
-          <t>350.000</t>
-        </is>
-      </c>
-      <c r="F67" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G67" s="7" t="inlineStr">
-        <is>
-          <t>150.000</t>
-        </is>
-      </c>
-      <c r="H67" s="6" t="inlineStr">
-        <is>
-          <t>Yola</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="6" t="inlineStr">
-        <is>
-          <t>TF0075</t>
-        </is>
-      </c>
-      <c r="B68" s="6" t="inlineStr">
-        <is>
-          <t>15-06-2025 15:09:27</t>
-        </is>
-      </c>
-      <c r="C68" s="6" t="inlineStr">
-        <is>
-          <t>M019</t>
-        </is>
-      </c>
-      <c r="D68" s="6" t="inlineStr">
-        <is>
-          <t>Paket Jamail</t>
-        </is>
-      </c>
-      <c r="E68" s="7" t="inlineStr">
-        <is>
-          <t>350.000</t>
-        </is>
-      </c>
-      <c r="F68" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G68" s="7" t="inlineStr">
-        <is>
-          <t>150.000</t>
-        </is>
-      </c>
-      <c r="H68" s="6" t="inlineStr">
-        <is>
-          <t>Yola</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="6" t="inlineStr">
-        <is>
-          <t>TF0076</t>
-        </is>
-      </c>
-      <c r="B69" s="6" t="inlineStr">
-        <is>
-          <t>15-06-2025 15:13:13</t>
-        </is>
-      </c>
-      <c r="C69" s="6" t="inlineStr">
-        <is>
-          <t>M019</t>
-        </is>
-      </c>
-      <c r="D69" s="6" t="inlineStr">
-        <is>
-          <t>Paket Jamail</t>
-        </is>
-      </c>
-      <c r="E69" s="7" t="inlineStr">
-        <is>
-          <t>350.000</t>
-        </is>
-      </c>
-      <c r="F69" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G69" s="7" t="inlineStr">
-        <is>
-          <t>150.000</t>
-        </is>
-      </c>
-      <c r="H69" s="6" t="inlineStr">
-        <is>
-          <t>Yola</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="6" t="inlineStr">
-        <is>
-          <t>TF0077</t>
-        </is>
-      </c>
-      <c r="B70" s="6" t="inlineStr">
-        <is>
-          <t>15-06-2025 15:14:34</t>
-        </is>
-      </c>
-      <c r="C70" s="6" t="inlineStr">
-        <is>
-          <t>M019</t>
-        </is>
-      </c>
-      <c r="D70" s="6" t="inlineStr">
-        <is>
-          <t>Paket Jamail</t>
-        </is>
-      </c>
-      <c r="E70" s="7" t="inlineStr">
-        <is>
-          <t>350.000</t>
-        </is>
-      </c>
-      <c r="F70" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G70" s="7" t="inlineStr">
-        <is>
-          <t>150.000</t>
-        </is>
-      </c>
-      <c r="H70" s="6" t="inlineStr">
-        <is>
-          <t>Yola</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="6" t="inlineStr">
-        <is>
-          <t>TF0078</t>
-        </is>
-      </c>
-      <c r="B71" s="6" t="inlineStr">
-        <is>
-          <t>15-06-2025 15:16:46</t>
-        </is>
-      </c>
-      <c r="C71" s="6" t="inlineStr">
-        <is>
-          <t>M002</t>
-        </is>
-      </c>
-      <c r="D71" s="6" t="inlineStr">
-        <is>
-          <t>Paket Sejahteramana</t>
-        </is>
-      </c>
-      <c r="E71" s="7" t="inlineStr">
-        <is>
-          <t>500.000</t>
-        </is>
-      </c>
-      <c r="F71" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G71" s="7" t="inlineStr">
-        <is>
-          <t>400.000</t>
-        </is>
-      </c>
-      <c r="H71" s="6" t="inlineStr">
-        <is>
-          <t>Yola</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="9" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="B72" s="6" t="n"/>
-      <c r="C72" s="6" t="n"/>
-      <c r="D72" s="6" t="n"/>
-      <c r="E72" s="6" t="n"/>
-      <c r="F72" s="9" t="inlineStr"/>
-      <c r="G72" s="10" t="inlineStr">
-        <is>
-          <t>4.775.000</t>
-        </is>
-      </c>
-      <c r="H72" s="9" t="inlineStr"/>
-    </row>
-    <row r="75">
-      <c r="A75" s="5" t="inlineStr">
+      <c r="A66" s="5" t="inlineStr">
         <is>
           <t>TOTAL SELURUH KOMISI</t>
         </is>
       </c>
-      <c r="B75" s="5" t="n"/>
-      <c r="C75" s="5" t="inlineStr"/>
-      <c r="D75" s="5" t="inlineStr"/>
-      <c r="E75" s="5" t="inlineStr"/>
-      <c r="F75" s="5" t="inlineStr"/>
-      <c r="G75" s="5" t="inlineStr">
-        <is>
-          <t>23.225.000</t>
-        </is>
-      </c>
-      <c r="H75" s="11" t="n"/>
+      <c r="B66" s="5" t="n"/>
+      <c r="C66" s="5" t="inlineStr"/>
+      <c r="D66" s="5" t="inlineStr"/>
+      <c r="E66" s="5" t="inlineStr"/>
+      <c r="F66" s="5" t="inlineStr"/>
+      <c r="G66" s="5" t="inlineStr">
+        <is>
+          <t>15.890.000</t>
+        </is>
+      </c>
+      <c r="H66" s="11" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="A50:E50"/>
-    <mergeCell ref="A72:E72"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A15:E15"/>
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A63:E63"/>
+    <mergeCell ref="A66:B66"/>
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
memunculkan nama terapis additional di list dan munculkan nama terapis di report, memunculkan harga ruangan di list dan di report juga
</commit_message>
<xml_diff>
--- a/datakomisiterapisbulanan.xlsx
+++ b/datakomisiterapisbulanan.xlsx
@@ -465,7 +465,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,7 +476,7 @@
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="33.6" customWidth="1" min="4" max="4"/>
+    <col width="27.6" customWidth="1" min="4" max="4"/>
     <col width="15.6" customWidth="1" min="5" max="5"/>
     <col width="7.199999999999999" customWidth="1" min="6" max="6"/>
     <col width="13.2" customWidth="1" min="7" max="7"/>
@@ -500,7 +500,7 @@
     <row r="2" ht="30" customHeight="1">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>LAPORAN KOMISI TERAPIS BULAN 8 TAHUN 2025</t>
+          <t>LAPORAN KOMISI TERAPIS BULAN 9 TAHUN 2025</t>
         </is>
       </c>
       <c r="B2" s="4" t="n"/>
@@ -562,7 +562,7 @@
       </c>
       <c r="B5" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Lola</t>
         </is>
       </c>
       <c r="C5" s="6" t="n"/>
@@ -575,27 +575,27 @@
     <row r="6">
       <c r="A6" s="6" t="inlineStr">
         <is>
-          <t>TF0163</t>
+          <t>TF0164</t>
         </is>
       </c>
       <c r="B6" s="6" t="inlineStr">
         <is>
-          <t>31-08-2025 18:26:59</t>
+          <t>01-09-2025 11:18:34</t>
         </is>
       </c>
       <c r="C6" s="6" t="inlineStr">
         <is>
-          <t>P002</t>
+          <t>M002</t>
         </is>
       </c>
       <c r="D6" s="6" t="inlineStr">
         <is>
-          <t>Hot Massage</t>
+          <t>Paket Sejahteramana</t>
         </is>
       </c>
       <c r="E6" s="7" t="inlineStr">
         <is>
-          <t>300.000</t>
+          <t>500.000</t>
         </is>
       </c>
       <c r="F6" s="8" t="n">
@@ -603,39 +603,39 @@
       </c>
       <c r="G6" s="7" t="inlineStr">
         <is>
-          <t>30.000</t>
+          <t>400.000</t>
         </is>
       </c>
       <c r="H6" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Lola</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="inlineStr">
         <is>
-          <t>TF0163</t>
+          <t>TF0164</t>
         </is>
       </c>
       <c r="B7" s="6" t="inlineStr">
         <is>
-          <t>31-08-2025 18:26:59</t>
+          <t>01-09-2025 11:18:34</t>
         </is>
       </c>
       <c r="C7" s="6" t="inlineStr">
         <is>
-          <t>P001</t>
+          <t>M003</t>
         </is>
       </c>
       <c r="D7" s="6" t="inlineStr">
         <is>
-          <t>Traditional Massage 30 Min</t>
+          <t>kalomania</t>
         </is>
       </c>
       <c r="E7" s="7" t="inlineStr">
         <is>
-          <t>200.000</t>
+          <t>500.000</t>
         </is>
       </c>
       <c r="F7" s="8" t="n">
@@ -643,24 +643,24 @@
       </c>
       <c r="G7" s="7" t="inlineStr">
         <is>
-          <t>20.000</t>
+          <t>225.000</t>
         </is>
       </c>
       <c r="H7" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Lola</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>TF0163</t>
+          <t>TF0165</t>
         </is>
       </c>
       <c r="B8" s="6" t="inlineStr">
         <is>
-          <t>31-08-2025 18:26:59</t>
+          <t>02-09-2025 12:51:03</t>
         </is>
       </c>
       <c r="C8" s="6" t="inlineStr">
@@ -688,19 +688,19 @@
       </c>
       <c r="H8" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Lola</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>TF0163</t>
+          <t>TF0165</t>
         </is>
       </c>
       <c r="B9" s="6" t="inlineStr">
         <is>
-          <t>31-08-2025 18:26:59</t>
+          <t>02-09-2025 12:51:03</t>
         </is>
       </c>
       <c r="C9" s="6" t="inlineStr">
@@ -728,19 +728,19 @@
       </c>
       <c r="H9" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Lola</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>TF0163</t>
+          <t>TF0165</t>
         </is>
       </c>
       <c r="B10" s="6" t="inlineStr">
         <is>
-          <t>31-08-2025 18:26:59</t>
+          <t>02-09-2025 12:51:03</t>
         </is>
       </c>
       <c r="C10" s="6" t="inlineStr">
@@ -768,145 +768,145 @@
       </c>
       <c r="H10" s="6" t="inlineStr">
         <is>
-          <t>Sasa</t>
+          <t>Lola</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="9" t="inlineStr">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>TF0165</t>
+        </is>
+      </c>
+      <c r="B11" s="6" t="inlineStr">
+        <is>
+          <t>02-09-2025 12:51:03</t>
+        </is>
+      </c>
+      <c r="C11" s="6" t="inlineStr">
+        <is>
+          <t>M001</t>
+        </is>
+      </c>
+      <c r="D11" s="6" t="inlineStr">
+        <is>
+          <t>paket holiday</t>
+        </is>
+      </c>
+      <c r="E11" s="7" t="inlineStr">
+        <is>
+          <t>550.000</t>
+        </is>
+      </c>
+      <c r="F11" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="7" t="inlineStr">
+        <is>
+          <t>275.000</t>
+        </is>
+      </c>
+      <c r="H11" s="6" t="inlineStr">
+        <is>
+          <t>Lola</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>TF0165</t>
+        </is>
+      </c>
+      <c r="B12" s="6" t="inlineStr">
+        <is>
+          <t>02-09-2025 12:51:03</t>
+        </is>
+      </c>
+      <c r="C12" s="6" t="inlineStr">
+        <is>
+          <t>M003</t>
+        </is>
+      </c>
+      <c r="D12" s="6" t="inlineStr">
+        <is>
+          <t>kalomania</t>
+        </is>
+      </c>
+      <c r="E12" s="7" t="inlineStr">
+        <is>
+          <t>500.000</t>
+        </is>
+      </c>
+      <c r="F12" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="7" t="inlineStr">
+        <is>
+          <t>450.000</t>
+        </is>
+      </c>
+      <c r="H12" s="6" t="inlineStr">
+        <is>
+          <t>Lola</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="9" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B11" s="6" t="n"/>
-      <c r="C11" s="6" t="n"/>
-      <c r="D11" s="6" t="n"/>
-      <c r="E11" s="6" t="n"/>
-      <c r="F11" s="9" t="inlineStr"/>
-      <c r="G11" s="10" t="inlineStr">
-        <is>
-          <t>1.075.000</t>
-        </is>
-      </c>
-      <c r="H11" s="9" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="6" t="n"/>
-      <c r="B12" s="6" t="n"/>
-      <c r="C12" s="6" t="n"/>
-      <c r="D12" s="6" t="n"/>
-      <c r="E12" s="6" t="n"/>
-      <c r="F12" s="6" t="n"/>
-      <c r="G12" s="6" t="n"/>
-      <c r="H12" s="6" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="inlineStr">
-        <is>
-          <t>Terapis :</t>
-        </is>
-      </c>
-      <c r="B13" s="6" t="inlineStr">
-        <is>
-          <t>Yola</t>
-        </is>
-      </c>
+      <c r="B13" s="6" t="n"/>
       <c r="C13" s="6" t="n"/>
       <c r="D13" s="6" t="n"/>
       <c r="E13" s="6" t="n"/>
-      <c r="F13" s="6" t="n"/>
-      <c r="G13" s="6" t="n"/>
-      <c r="H13" s="6" t="n"/>
+      <c r="F13" s="9" t="inlineStr"/>
+      <c r="G13" s="10" t="inlineStr">
+        <is>
+          <t>2.375.000</t>
+        </is>
+      </c>
+      <c r="H13" s="9" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" s="6" t="inlineStr">
-        <is>
-          <t>TF0163</t>
-        </is>
-      </c>
-      <c r="B14" s="6" t="inlineStr">
-        <is>
-          <t>31-08-2025 18:26:59</t>
-        </is>
-      </c>
-      <c r="C14" s="6" t="inlineStr">
-        <is>
-          <t>P002</t>
-        </is>
-      </c>
-      <c r="D14" s="6" t="inlineStr">
-        <is>
-          <t>Hot Massage</t>
-        </is>
-      </c>
-      <c r="E14" s="7" t="inlineStr">
-        <is>
-          <t>300.000</t>
-        </is>
-      </c>
-      <c r="F14" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G14" s="7" t="inlineStr">
-        <is>
-          <t>30.000</t>
-        </is>
-      </c>
-      <c r="H14" s="6" t="inlineStr">
-        <is>
-          <t>Yola</t>
-        </is>
-      </c>
+      <c r="A14" s="6" t="n"/>
+      <c r="B14" s="6" t="n"/>
+      <c r="C14" s="6" t="n"/>
+      <c r="D14" s="6" t="n"/>
+      <c r="E14" s="6" t="n"/>
+      <c r="F14" s="6" t="n"/>
+      <c r="G14" s="6" t="n"/>
+      <c r="H14" s="6" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="6" t="inlineStr">
         <is>
-          <t>TF0163</t>
+          <t>Terapis :</t>
         </is>
       </c>
       <c r="B15" s="6" t="inlineStr">
         <is>
-          <t>31-08-2025 18:26:59</t>
-        </is>
-      </c>
-      <c r="C15" s="6" t="inlineStr">
-        <is>
-          <t>P001</t>
-        </is>
-      </c>
-      <c r="D15" s="6" t="inlineStr">
-        <is>
-          <t>Traditional Massage 30 Min</t>
-        </is>
-      </c>
-      <c r="E15" s="7" t="inlineStr">
-        <is>
-          <t>200.000</t>
-        </is>
-      </c>
-      <c r="F15" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G15" s="7" t="inlineStr">
-        <is>
-          <t>20.000</t>
-        </is>
-      </c>
-      <c r="H15" s="6" t="inlineStr">
-        <is>
-          <t>Yola</t>
-        </is>
-      </c>
+          <t>Sasa</t>
+        </is>
+      </c>
+      <c r="C15" s="6" t="n"/>
+      <c r="D15" s="6" t="n"/>
+      <c r="E15" s="6" t="n"/>
+      <c r="F15" s="6" t="n"/>
+      <c r="G15" s="6" t="n"/>
+      <c r="H15" s="6" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="6" t="inlineStr">
         <is>
-          <t>TF0163</t>
+          <t>TF0165</t>
         </is>
       </c>
       <c r="B16" s="6" t="inlineStr">
         <is>
-          <t>31-08-2025 18:26:59</t>
+          <t>02-09-2025 12:51:03</t>
         </is>
       </c>
       <c r="C16" s="6" t="inlineStr">
@@ -934,19 +934,19 @@
       </c>
       <c r="H16" s="6" t="inlineStr">
         <is>
-          <t>Yola</t>
+          <t>Sasa</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="6" t="inlineStr">
         <is>
-          <t>TF0163</t>
+          <t>TF0165</t>
         </is>
       </c>
       <c r="B17" s="6" t="inlineStr">
         <is>
-          <t>31-08-2025 18:26:59</t>
+          <t>02-09-2025 12:51:03</t>
         </is>
       </c>
       <c r="C17" s="6" t="inlineStr">
@@ -974,19 +974,19 @@
       </c>
       <c r="H17" s="6" t="inlineStr">
         <is>
-          <t>Yola</t>
+          <t>Sasa</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="inlineStr">
         <is>
-          <t>TF0163</t>
+          <t>TF0165</t>
         </is>
       </c>
       <c r="B18" s="6" t="inlineStr">
         <is>
-          <t>31-08-2025 18:26:59</t>
+          <t>02-09-2025 12:51:03</t>
         </is>
       </c>
       <c r="C18" s="6" t="inlineStr">
@@ -1014,53 +1014,460 @@
       </c>
       <c r="H18" s="6" t="inlineStr">
         <is>
+          <t>Sasa</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="inlineStr">
+        <is>
+          <t>TF0165</t>
+        </is>
+      </c>
+      <c r="B19" s="6" t="inlineStr">
+        <is>
+          <t>02-09-2025 12:51:03</t>
+        </is>
+      </c>
+      <c r="C19" s="6" t="inlineStr">
+        <is>
+          <t>M001</t>
+        </is>
+      </c>
+      <c r="D19" s="6" t="inlineStr">
+        <is>
+          <t>paket holiday</t>
+        </is>
+      </c>
+      <c r="E19" s="7" t="inlineStr">
+        <is>
+          <t>550.000</t>
+        </is>
+      </c>
+      <c r="F19" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" s="7" t="inlineStr">
+        <is>
+          <t>275.000</t>
+        </is>
+      </c>
+      <c r="H19" s="6" t="inlineStr">
+        <is>
+          <t>Sasa</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>TF0165</t>
+        </is>
+      </c>
+      <c r="B20" s="6" t="inlineStr">
+        <is>
+          <t>02-09-2025 12:51:03</t>
+        </is>
+      </c>
+      <c r="C20" s="6" t="inlineStr">
+        <is>
+          <t>M003</t>
+        </is>
+      </c>
+      <c r="D20" s="6" t="inlineStr">
+        <is>
+          <t>kalomania</t>
+        </is>
+      </c>
+      <c r="E20" s="7" t="inlineStr">
+        <is>
+          <t>500.000</t>
+        </is>
+      </c>
+      <c r="F20" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="G20" s="7" t="inlineStr">
+        <is>
+          <t>450.000</t>
+        </is>
+      </c>
+      <c r="H20" s="6" t="inlineStr">
+        <is>
+          <t>Sasa</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="9" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="B21" s="6" t="n"/>
+      <c r="C21" s="6" t="n"/>
+      <c r="D21" s="6" t="n"/>
+      <c r="E21" s="6" t="n"/>
+      <c r="F21" s="9" t="inlineStr"/>
+      <c r="G21" s="10" t="inlineStr">
+        <is>
+          <t>1.750.000</t>
+        </is>
+      </c>
+      <c r="H21" s="9" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="n"/>
+      <c r="B22" s="6" t="n"/>
+      <c r="C22" s="6" t="n"/>
+      <c r="D22" s="6" t="n"/>
+      <c r="E22" s="6" t="n"/>
+      <c r="F22" s="6" t="n"/>
+      <c r="G22" s="6" t="n"/>
+      <c r="H22" s="6" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="inlineStr">
+        <is>
+          <t>Terapis :</t>
+        </is>
+      </c>
+      <c r="B23" s="6" t="inlineStr">
+        <is>
           <t>Yola</t>
         </is>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="9" t="inlineStr">
+      <c r="C23" s="6" t="n"/>
+      <c r="D23" s="6" t="n"/>
+      <c r="E23" s="6" t="n"/>
+      <c r="F23" s="6" t="n"/>
+      <c r="G23" s="6" t="n"/>
+      <c r="H23" s="6" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="inlineStr">
+        <is>
+          <t>TF0164</t>
+        </is>
+      </c>
+      <c r="B24" s="6" t="inlineStr">
+        <is>
+          <t>01-09-2025 11:18:34</t>
+        </is>
+      </c>
+      <c r="C24" s="6" t="inlineStr">
+        <is>
+          <t>M002</t>
+        </is>
+      </c>
+      <c r="D24" s="6" t="inlineStr">
+        <is>
+          <t>Paket Sejahteramana</t>
+        </is>
+      </c>
+      <c r="E24" s="7" t="inlineStr">
+        <is>
+          <t>500.000</t>
+        </is>
+      </c>
+      <c r="F24" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G24" s="7" t="inlineStr">
+        <is>
+          <t>400.000</t>
+        </is>
+      </c>
+      <c r="H24" s="6" t="inlineStr">
+        <is>
+          <t>Yola</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="inlineStr">
+        <is>
+          <t>TF0164</t>
+        </is>
+      </c>
+      <c r="B25" s="6" t="inlineStr">
+        <is>
+          <t>01-09-2025 11:18:34</t>
+        </is>
+      </c>
+      <c r="C25" s="6" t="inlineStr">
+        <is>
+          <t>M003</t>
+        </is>
+      </c>
+      <c r="D25" s="6" t="inlineStr">
+        <is>
+          <t>kalomania</t>
+        </is>
+      </c>
+      <c r="E25" s="7" t="inlineStr">
+        <is>
+          <t>500.000</t>
+        </is>
+      </c>
+      <c r="F25" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G25" s="7" t="inlineStr">
+        <is>
+          <t>225.000</t>
+        </is>
+      </c>
+      <c r="H25" s="6" t="inlineStr">
+        <is>
+          <t>Yola</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="inlineStr">
+        <is>
+          <t>TF0165</t>
+        </is>
+      </c>
+      <c r="B26" s="6" t="inlineStr">
+        <is>
+          <t>02-09-2025 12:51:03</t>
+        </is>
+      </c>
+      <c r="C26" s="6" t="inlineStr">
+        <is>
+          <t>M003</t>
+        </is>
+      </c>
+      <c r="D26" s="6" t="inlineStr">
+        <is>
+          <t>kalomania</t>
+        </is>
+      </c>
+      <c r="E26" s="7" t="inlineStr">
+        <is>
+          <t>500.000</t>
+        </is>
+      </c>
+      <c r="F26" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G26" s="7" t="inlineStr">
+        <is>
+          <t>225.000</t>
+        </is>
+      </c>
+      <c r="H26" s="6" t="inlineStr">
+        <is>
+          <t>Yola</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="6" t="inlineStr">
+        <is>
+          <t>TF0165</t>
+        </is>
+      </c>
+      <c r="B27" s="6" t="inlineStr">
+        <is>
+          <t>02-09-2025 12:51:03</t>
+        </is>
+      </c>
+      <c r="C27" s="6" t="inlineStr">
+        <is>
+          <t>M002</t>
+        </is>
+      </c>
+      <c r="D27" s="6" t="inlineStr">
+        <is>
+          <t>Paket Sejahteramana</t>
+        </is>
+      </c>
+      <c r="E27" s="7" t="inlineStr">
+        <is>
+          <t>500.000</t>
+        </is>
+      </c>
+      <c r="F27" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" s="7" t="inlineStr">
+        <is>
+          <t>400.000</t>
+        </is>
+      </c>
+      <c r="H27" s="6" t="inlineStr">
+        <is>
+          <t>Yola</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="inlineStr">
+        <is>
+          <t>TF0165</t>
+        </is>
+      </c>
+      <c r="B28" s="6" t="inlineStr">
+        <is>
+          <t>02-09-2025 12:51:03</t>
+        </is>
+      </c>
+      <c r="C28" s="6" t="inlineStr">
+        <is>
+          <t>M004</t>
+        </is>
+      </c>
+      <c r="D28" s="6" t="inlineStr">
+        <is>
+          <t>paket bajinurakaloman</t>
+        </is>
+      </c>
+      <c r="E28" s="7" t="inlineStr">
+        <is>
+          <t>4.000.000</t>
+        </is>
+      </c>
+      <c r="F28" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" s="7" t="inlineStr">
+        <is>
+          <t>400.000</t>
+        </is>
+      </c>
+      <c r="H28" s="6" t="inlineStr">
+        <is>
+          <t>Yola</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="inlineStr">
+        <is>
+          <t>TF0165</t>
+        </is>
+      </c>
+      <c r="B29" s="6" t="inlineStr">
+        <is>
+          <t>02-09-2025 12:51:03</t>
+        </is>
+      </c>
+      <c r="C29" s="6" t="inlineStr">
+        <is>
+          <t>M001</t>
+        </is>
+      </c>
+      <c r="D29" s="6" t="inlineStr">
+        <is>
+          <t>paket holiday</t>
+        </is>
+      </c>
+      <c r="E29" s="7" t="inlineStr">
+        <is>
+          <t>550.000</t>
+        </is>
+      </c>
+      <c r="F29" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="7" t="inlineStr">
+        <is>
+          <t>275.000</t>
+        </is>
+      </c>
+      <c r="H29" s="6" t="inlineStr">
+        <is>
+          <t>Yola</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="inlineStr">
+        <is>
+          <t>TF0165</t>
+        </is>
+      </c>
+      <c r="B30" s="6" t="inlineStr">
+        <is>
+          <t>02-09-2025 12:51:03</t>
+        </is>
+      </c>
+      <c r="C30" s="6" t="inlineStr">
+        <is>
+          <t>M003</t>
+        </is>
+      </c>
+      <c r="D30" s="6" t="inlineStr">
+        <is>
+          <t>kalomania</t>
+        </is>
+      </c>
+      <c r="E30" s="7" t="inlineStr">
+        <is>
+          <t>500.000</t>
+        </is>
+      </c>
+      <c r="F30" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="G30" s="7" t="inlineStr">
+        <is>
+          <t>450.000</t>
+        </is>
+      </c>
+      <c r="H30" s="6" t="inlineStr">
+        <is>
+          <t>Yola</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="9" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B19" s="6" t="n"/>
-      <c r="C19" s="6" t="n"/>
-      <c r="D19" s="6" t="n"/>
-      <c r="E19" s="6" t="n"/>
-      <c r="F19" s="9" t="inlineStr"/>
-      <c r="G19" s="10" t="inlineStr">
-        <is>
-          <t>1.075.000</t>
-        </is>
-      </c>
-      <c r="H19" s="9" t="inlineStr"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="5" t="inlineStr">
+      <c r="B31" s="6" t="n"/>
+      <c r="C31" s="6" t="n"/>
+      <c r="D31" s="6" t="n"/>
+      <c r="E31" s="6" t="n"/>
+      <c r="F31" s="9" t="inlineStr"/>
+      <c r="G31" s="10" t="inlineStr">
+        <is>
+          <t>2.375.000</t>
+        </is>
+      </c>
+      <c r="H31" s="9" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="5" t="inlineStr">
         <is>
           <t>TOTAL SELURUH KOMISI</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="inlineStr"/>
-      <c r="D22" s="5" t="inlineStr"/>
-      <c r="E22" s="5" t="inlineStr"/>
-      <c r="F22" s="5" t="inlineStr"/>
-      <c r="G22" s="5" t="inlineStr">
-        <is>
-          <t>2.150.000</t>
-        </is>
-      </c>
-      <c r="H22" s="11" t="n"/>
+      <c r="B34" s="5" t="n"/>
+      <c r="C34" s="5" t="inlineStr"/>
+      <c r="D34" s="5" t="inlineStr"/>
+      <c r="E34" s="5" t="inlineStr"/>
+      <c r="F34" s="5" t="inlineStr"/>
+      <c r="G34" s="5" t="inlineStr">
+        <is>
+          <t>6.500.000</t>
+        </is>
+      </c>
+      <c r="H34" s="11" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A34:B34"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>